<commit_message>
Añadido el modo de light sleep
</commit_message>
<xml_diff>
--- a/Datasheets/ESP CONTROLADOR.xlsx
+++ b/Datasheets/ESP CONTROLADOR.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uses0-my.sharepoint.com/personal/serparram_alum_us_es/Documents/Escritorio/Tercero/SegundoCuatri/Proyectos integrados/Datasheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uses0-my.sharepoint.com/personal/serparram_alum_us_es/Documents/Escritorio/Tercero/SegundoCuatri/Proyectos integrados/pi01/Datasheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="64" documentId="8_{D3A0FABF-8483-46B0-83EF-1E4F1725AC99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{90462375-39B1-4BCB-9994-D8958D33FF95}"/>
+  <xr:revisionPtr revIDLastSave="65" documentId="8_{D3A0FABF-8483-46B0-83EF-1E4F1725AC99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1356C05F-44BE-4F49-AA7D-E21B0511569E}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{121CA96C-2885-4729-A560-A640673F77D6}"/>
   </bookViews>
@@ -36,15 +36,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="108">
   <si>
     <t>INPUT</t>
   </si>
   <si>
     <t>OUTPUT</t>
-  </si>
-  <si>
-    <t>WIFI</t>
   </si>
   <si>
     <t>GPIO</t>
@@ -697,21 +694,51 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -736,41 +763,11 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -787,6 +784,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1109,7 +1110,7 @@
   <dimension ref="A1:P83"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13:M17"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1127,10 +1128,10 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>0</v>
@@ -1139,30 +1140,30 @@
         <v>1</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="7" t="s">
-        <v>18</v>
-      </c>
       <c r="I1" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="K1" s="7" t="s">
         <v>72</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>73</v>
       </c>
       <c r="L1" s="1"/>
       <c r="M1" s="9"/>
       <c r="N1" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
@@ -1171,22 +1172,22 @@
       <c r="A2" s="8">
         <v>1</v>
       </c>
-      <c r="B2" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
+      <c r="B2" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
       <c r="L2" s="1"/>
       <c r="M2" s="2"/>
       <c r="N2" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
@@ -1195,22 +1196,22 @@
       <c r="A3" s="8">
         <v>2</v>
       </c>
-      <c r="B3" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="31"/>
-      <c r="I3" s="31"/>
-      <c r="J3" s="31"/>
-      <c r="K3" s="31"/>
+      <c r="B3" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
       <c r="L3" s="1"/>
       <c r="M3" s="3"/>
       <c r="N3" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
@@ -1219,18 +1220,18 @@
       <c r="A4" s="8">
         <v>3</v>
       </c>
-      <c r="B4" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="21"/>
-      <c r="K4" s="21"/>
+      <c r="B4" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="29"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
@@ -1244,25 +1245,25 @@
       <c r="B5" s="1">
         <v>36</v>
       </c>
-      <c r="C5" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="19"/>
+      <c r="C5" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="26"/>
       <c r="E5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
-      <c r="K5" s="32" t="s">
-        <v>92</v>
+      <c r="K5" s="17" t="s">
+        <v>91</v>
       </c>
       <c r="L5" s="1"/>
-      <c r="M5" s="41" t="s">
-        <v>108</v>
+      <c r="M5" s="24" t="s">
+        <v>107</v>
       </c>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
@@ -1275,25 +1276,25 @@
       <c r="B6" s="1">
         <v>39</v>
       </c>
-      <c r="C6" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="19"/>
+      <c r="C6" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="26"/>
       <c r="E6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
-      <c r="K6" s="32" t="s">
-        <v>93</v>
+      <c r="K6" s="17" t="s">
+        <v>92</v>
       </c>
       <c r="L6" s="1"/>
       <c r="M6" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
@@ -1306,23 +1307,23 @@
       <c r="B7" s="1">
         <v>34</v>
       </c>
-      <c r="C7" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="19"/>
+      <c r="C7" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="26"/>
       <c r="E7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
-      <c r="K7" s="32"/>
+      <c r="K7" s="17"/>
       <c r="L7" s="1"/>
       <c r="M7" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
@@ -1335,20 +1336,20 @@
       <c r="B8" s="1">
         <v>35</v>
       </c>
-      <c r="C8" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="19"/>
+      <c r="C8" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="26"/>
       <c r="E8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
-      <c r="K8" s="32"/>
+      <c r="K8" s="17"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
@@ -1363,24 +1364,24 @@
         <v>32</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I9" s="1"/>
-      <c r="K9" s="32" t="s">
-        <v>94</v>
+      <c r="K9" s="17" t="s">
+        <v>93</v>
       </c>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
@@ -1396,24 +1397,24 @@
         <v>33</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I10" s="1"/>
-      <c r="K10" s="39" t="s">
-        <v>105</v>
+      <c r="K10" s="22" t="s">
+        <v>104</v>
       </c>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
@@ -1429,23 +1430,23 @@
         <v>25</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
-      <c r="K11" s="34"/>
+      <c r="K11" s="19"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
       <c r="O11" s="1"/>
@@ -1459,27 +1460,27 @@
         <v>26</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
-      <c r="K12" s="34"/>
+      <c r="K12" s="19"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
       <c r="N12" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="O12" s="14" t="s">
         <v>0</v>
@@ -1494,32 +1495,32 @@
         <v>27</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
-      <c r="K13" s="34" t="s">
-        <v>101</v>
+      <c r="K13" s="19" t="s">
+        <v>100</v>
       </c>
       <c r="L13" s="1"/>
-      <c r="M13" s="17" t="s">
-        <v>89</v>
+      <c r="M13" s="30" t="s">
+        <v>88</v>
       </c>
       <c r="N13" s="13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="O13" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="P13" s="1"/>
     </row>
@@ -1531,32 +1532,32 @@
         <v>14</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="K14" s="34"/>
+        <v>67</v>
+      </c>
+      <c r="K14" s="19"/>
       <c r="L14" s="1"/>
-      <c r="M14" s="17"/>
+      <c r="M14" s="30"/>
       <c r="N14" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="P14" s="1"/>
     </row>
@@ -1568,35 +1569,35 @@
         <v>12</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="K15" s="34"/>
+        <v>74</v>
+      </c>
+      <c r="K15" s="19"/>
       <c r="L15" s="1"/>
-      <c r="M15" s="17"/>
+      <c r="M15" s="30"/>
       <c r="N15" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O15" s="13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="P15" s="1"/>
     </row>
@@ -1604,25 +1605,25 @@
       <c r="A16" s="8">
         <v>15</v>
       </c>
-      <c r="B16" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="20"/>
-      <c r="J16" s="20"/>
-      <c r="K16" s="20"/>
+      <c r="B16" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="31"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="31"/>
+      <c r="G16" s="31"/>
+      <c r="H16" s="31"/>
+      <c r="I16" s="31"/>
+      <c r="J16" s="31"/>
+      <c r="K16" s="31"/>
       <c r="L16" s="1"/>
-      <c r="M16" s="17"/>
+      <c r="M16" s="30"/>
       <c r="N16" s="13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="O16" s="13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="P16" s="1"/>
     </row>
@@ -1634,32 +1635,32 @@
         <v>13</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H17" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H17" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="I17" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="K17" s="33"/>
+        <v>69</v>
+      </c>
+      <c r="K17" s="18"/>
       <c r="L17" s="1"/>
-      <c r="M17" s="17"/>
+      <c r="M17" s="30"/>
       <c r="N17" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="O17" s="40" t="s">
-        <v>91</v>
+        <v>85</v>
+      </c>
+      <c r="O17" s="23" t="s">
+        <v>90</v>
       </c>
       <c r="P17" s="1"/>
     </row>
@@ -1670,20 +1671,20 @@
       <c r="B18" s="1">
         <v>9</v>
       </c>
-      <c r="C18" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18" s="24"/>
+      <c r="C18" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="34"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
-      <c r="J18" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="K18" s="29" t="s">
-        <v>9</v>
+      <c r="J18" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="K18" s="39" t="s">
+        <v>8</v>
       </c>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
@@ -1702,15 +1703,15 @@
       <c r="B19" s="1">
         <v>10</v>
       </c>
-      <c r="C19" s="25"/>
-      <c r="D19" s="26"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="36"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
-      <c r="J19" s="22"/>
-      <c r="K19" s="29"/>
+      <c r="J19" s="32"/>
+      <c r="K19" s="39"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
@@ -1724,15 +1725,15 @@
       <c r="B20" s="1">
         <v>11</v>
       </c>
-      <c r="C20" s="25"/>
-      <c r="D20" s="26"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="36"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
-      <c r="J20" s="22"/>
-      <c r="K20" s="29"/>
+      <c r="J20" s="32"/>
+      <c r="K20" s="39"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
@@ -1746,15 +1747,15 @@
       <c r="B21" s="1">
         <v>6</v>
       </c>
-      <c r="C21" s="25"/>
-      <c r="D21" s="26"/>
+      <c r="C21" s="35"/>
+      <c r="D21" s="36"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
-      <c r="J21" s="22"/>
-      <c r="K21" s="29"/>
+      <c r="J21" s="32"/>
+      <c r="K21" s="39"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
@@ -1768,15 +1769,15 @@
       <c r="B22" s="1">
         <v>7</v>
       </c>
-      <c r="C22" s="25"/>
-      <c r="D22" s="26"/>
+      <c r="C22" s="35"/>
+      <c r="D22" s="36"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
-      <c r="J22" s="22"/>
-      <c r="K22" s="29"/>
+      <c r="J22" s="32"/>
+      <c r="K22" s="39"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
@@ -1790,15 +1791,15 @@
       <c r="B23" s="1">
         <v>8</v>
       </c>
-      <c r="C23" s="27"/>
-      <c r="D23" s="28"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="38"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
-      <c r="J23" s="22"/>
-      <c r="K23" s="29"/>
+      <c r="J23" s="32"/>
+      <c r="K23" s="39"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
@@ -1812,26 +1813,26 @@
       <c r="B24" s="1">
         <v>15</v>
       </c>
-      <c r="C24" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="D24" s="35" t="s">
-        <v>8</v>
+      <c r="C24" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="20" t="s">
+        <v>7</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H24" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H24" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="I24" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="K24" s="34"/>
+        <v>66</v>
+      </c>
+      <c r="K24" s="19"/>
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
@@ -1845,24 +1846,24 @@
       <c r="B25" s="1">
         <v>2</v>
       </c>
-      <c r="C25" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="D25" s="35" t="s">
-        <v>8</v>
+      <c r="C25" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="20" t="s">
+        <v>7</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I25" s="1"/>
-      <c r="K25" s="34"/>
+      <c r="K25" s="19"/>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
@@ -1876,27 +1877,27 @@
       <c r="B26" s="10">
         <v>0</v>
       </c>
-      <c r="C26" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="D26" s="36" t="s">
-        <v>8</v>
+      <c r="C26" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="21" t="s">
+        <v>7</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F26" s="10"/>
       <c r="G26" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="H26" s="10" t="s">
         <v>54</v>
-      </c>
-      <c r="H26" s="10" t="s">
-        <v>55</v>
       </c>
       <c r="I26" s="10"/>
       <c r="J26" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="K26" s="34"/>
+        <v>75</v>
+      </c>
+      <c r="K26" s="19"/>
       <c r="L26" s="10"/>
       <c r="M26" s="10"/>
       <c r="N26" s="10"/>
@@ -1911,24 +1912,24 @@
         <v>4</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I27" s="1"/>
-      <c r="K27" s="34" t="s">
-        <v>102</v>
+      <c r="K27" s="19" t="s">
+        <v>101</v>
       </c>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
@@ -1944,18 +1945,18 @@
         <v>16</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
-      <c r="K28" s="34" t="s">
-        <v>104</v>
+      <c r="K28" s="19" t="s">
+        <v>103</v>
       </c>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
@@ -1971,18 +1972,18 @@
         <v>17</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
-      <c r="K29" s="34" t="s">
-        <v>95</v>
+      <c r="K29" s="19" t="s">
+        <v>94</v>
       </c>
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
@@ -1998,20 +1999,20 @@
         <v>5</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="K30" s="34" t="s">
-        <v>97</v>
+        <v>65</v>
+      </c>
+      <c r="K30" s="19" t="s">
+        <v>96</v>
       </c>
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
@@ -2027,20 +2028,20 @@
         <v>18</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="K31" s="34" t="s">
-        <v>98</v>
+        <v>62</v>
+      </c>
+      <c r="K31" s="19" t="s">
+        <v>97</v>
       </c>
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
@@ -2056,20 +2057,20 @@
         <v>19</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="K32" s="34" t="s">
-        <v>99</v>
+        <v>64</v>
+      </c>
+      <c r="K32" s="19" t="s">
+        <v>98</v>
       </c>
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
@@ -2081,18 +2082,18 @@
       <c r="A33" s="8">
         <v>32</v>
       </c>
-      <c r="B33" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
-      <c r="F33" s="21"/>
-      <c r="G33" s="21"/>
-      <c r="H33" s="21"/>
-      <c r="I33" s="21"/>
-      <c r="J33" s="21"/>
-      <c r="K33" s="21"/>
+      <c r="B33" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" s="29"/>
+      <c r="D33" s="29"/>
+      <c r="E33" s="29"/>
+      <c r="F33" s="29"/>
+      <c r="G33" s="29"/>
+      <c r="H33" s="29"/>
+      <c r="I33" s="29"/>
+      <c r="J33" s="29"/>
+      <c r="K33" s="29"/>
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
       <c r="N33" s="1"/>
@@ -2107,19 +2108,19 @@
         <v>21</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="K34" s="32"/>
+        <v>61</v>
+      </c>
+      <c r="K34" s="17"/>
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
       <c r="N34" s="1"/>
@@ -2134,23 +2135,23 @@
         <v>3</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K35" s="37" t="s">
-        <v>96</v>
+        <v>77</v>
+      </c>
+      <c r="K35" s="40" t="s">
+        <v>95</v>
       </c>
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
@@ -2166,22 +2167,22 @@
         <v>1</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
       <c r="I36" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="K36" s="38"/>
+        <v>78</v>
+      </c>
+      <c r="K36" s="41"/>
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
       <c r="N36" s="1"/>
@@ -2196,20 +2197,20 @@
         <v>22</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
       <c r="I37" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="K37" s="32" t="s">
-        <v>100</v>
+        <v>61</v>
+      </c>
+      <c r="K37" s="17" t="s">
+        <v>99</v>
       </c>
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
@@ -2225,20 +2226,20 @@
         <v>23</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
       <c r="I38" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="K38" s="32" t="s">
-        <v>103</v>
+        <v>63</v>
+      </c>
+      <c r="K38" s="17" t="s">
+        <v>102</v>
       </c>
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
@@ -2250,18 +2251,18 @@
       <c r="A39" s="8">
         <v>38</v>
       </c>
-      <c r="B39" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="C39" s="20"/>
-      <c r="D39" s="20"/>
-      <c r="E39" s="20"/>
-      <c r="F39" s="20"/>
-      <c r="G39" s="20"/>
-      <c r="H39" s="20"/>
-      <c r="I39" s="20"/>
-      <c r="J39" s="20"/>
-      <c r="K39" s="20"/>
+      <c r="B39" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="C39" s="31"/>
+      <c r="D39" s="31"/>
+      <c r="E39" s="31"/>
+      <c r="F39" s="31"/>
+      <c r="G39" s="31"/>
+      <c r="H39" s="31"/>
+      <c r="I39" s="31"/>
+      <c r="J39" s="31"/>
+      <c r="K39" s="31"/>
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
       <c r="N39" s="1"/>
@@ -3061,12 +3062,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="B2:K2"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="B4:K4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
     <mergeCell ref="M13:M17"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="B16:K16"/>
@@ -3076,6 +3071,12 @@
     <mergeCell ref="C18:D23"/>
     <mergeCell ref="K18:K23"/>
     <mergeCell ref="K35:K36"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="B2:K2"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="B4:K4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Añadido librerias OneWire y Dallas Temperature
</commit_message>
<xml_diff>
--- a/Datasheets/ESP CONTROLADOR.xlsx
+++ b/Datasheets/ESP CONTROLADOR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uses0-my.sharepoint.com/personal/serparram_alum_us_es/Documents/Escritorio/Tercero/SegundoCuatri/Proyectos integrados/pi01/Datasheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="65" documentId="8_{D3A0FABF-8483-46B0-83EF-1E4F1725AC99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1356C05F-44BE-4F49-AA7D-E21B0511569E}"/>
+  <xr:revisionPtr revIDLastSave="78" documentId="8_{D3A0FABF-8483-46B0-83EF-1E4F1725AC99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E8D103F8-0D86-434D-BF50-AC83C5DB5F82}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{121CA96C-2885-4729-A560-A640673F77D6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="111">
   <si>
     <t>INPUT</t>
   </si>
@@ -290,9 +290,6 @@
     <t>1 Motor mezcladora</t>
   </si>
   <si>
-    <t>2 valvulas</t>
-  </si>
-  <si>
     <t>6 ultrasonidos</t>
   </si>
   <si>
@@ -356,10 +353,22 @@
     <t>2 Input</t>
   </si>
   <si>
-    <t>9 I/O</t>
-  </si>
-  <si>
     <t>Libres</t>
+  </si>
+  <si>
+    <t>Valvula 3</t>
+  </si>
+  <si>
+    <t>3 valvulas</t>
+  </si>
+  <si>
+    <t>1 Bomba agua</t>
+  </si>
+  <si>
+    <t>Bomba agua</t>
+  </si>
+  <si>
+    <t>7 I/O</t>
   </si>
 </sst>
 </file>
@@ -644,7 +653,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -691,9 +700,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -718,57 +724,64 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1110,7 +1123,7 @@
   <dimension ref="A1:P83"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1172,18 +1185,18 @@
       <c r="A2" s="8">
         <v>1</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
       <c r="L2" s="1"/>
       <c r="M2" s="2"/>
       <c r="N2" s="1" t="s">
@@ -1196,18 +1209,18 @@
       <c r="A3" s="8">
         <v>2</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="40"/>
+      <c r="K3" s="40"/>
       <c r="L3" s="1"/>
       <c r="M3" s="3"/>
       <c r="N3" s="1" t="s">
@@ -1220,18 +1233,18 @@
       <c r="A4" s="8">
         <v>3</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="29"/>
-      <c r="K4" s="29"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="28"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
@@ -1258,12 +1271,12 @@
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
-      <c r="K5" s="17" t="s">
-        <v>91</v>
+      <c r="K5" s="16" t="s">
+        <v>90</v>
       </c>
       <c r="L5" s="1"/>
-      <c r="M5" s="24" t="s">
-        <v>107</v>
+      <c r="M5" s="23" t="s">
+        <v>105</v>
       </c>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
@@ -1289,12 +1302,12 @@
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
-      <c r="K6" s="17" t="s">
-        <v>92</v>
+      <c r="K6" s="16" t="s">
+        <v>91</v>
       </c>
       <c r="L6" s="1"/>
       <c r="M6" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
@@ -1320,10 +1333,10 @@
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
-      <c r="K7" s="17"/>
+      <c r="K7" s="16"/>
       <c r="L7" s="1"/>
       <c r="M7" s="13" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
@@ -1349,7 +1362,7 @@
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
-      <c r="K8" s="17"/>
+      <c r="K8" s="16"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
@@ -1380,8 +1393,8 @@
         <v>45</v>
       </c>
       <c r="I9" s="1"/>
-      <c r="K9" s="17" t="s">
-        <v>93</v>
+      <c r="K9" s="16" t="s">
+        <v>92</v>
       </c>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
@@ -1413,8 +1426,8 @@
         <v>44</v>
       </c>
       <c r="I10" s="1"/>
-      <c r="K10" s="22" t="s">
-        <v>104</v>
+      <c r="K10" s="21" t="s">
+        <v>103</v>
       </c>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
@@ -1446,7 +1459,7 @@
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
-      <c r="K11" s="19"/>
+      <c r="K11" s="18"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
       <c r="O11" s="1"/>
@@ -1476,7 +1489,7 @@
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
-      <c r="K12" s="19"/>
+      <c r="K12" s="18"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
       <c r="N12" s="15" t="s">
@@ -1509,18 +1522,18 @@
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
-      <c r="K13" s="19" t="s">
-        <v>100</v>
+      <c r="K13" s="18" t="s">
+        <v>99</v>
       </c>
       <c r="L13" s="1"/>
-      <c r="M13" s="30" t="s">
-        <v>88</v>
+      <c r="M13" s="24" t="s">
+        <v>87</v>
       </c>
       <c r="N13" s="13" t="s">
         <v>80</v>
       </c>
       <c r="O13" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="P13" s="1"/>
     </row>
@@ -1550,14 +1563,16 @@
       <c r="I14" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="K14" s="19"/>
+      <c r="K14" s="18" t="s">
+        <v>109</v>
+      </c>
       <c r="L14" s="1"/>
-      <c r="M14" s="30"/>
+      <c r="M14" s="24"/>
       <c r="N14" s="13" t="s">
         <v>82</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="P14" s="1"/>
     </row>
@@ -1590,14 +1605,14 @@
       <c r="J15" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="K15" s="19"/>
+      <c r="K15" s="18"/>
       <c r="L15" s="1"/>
-      <c r="M15" s="30"/>
+      <c r="M15" s="24"/>
       <c r="N15" s="13" t="s">
         <v>83</v>
       </c>
       <c r="O15" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="P15" s="1"/>
     </row>
@@ -1605,29 +1620,29 @@
       <c r="A16" s="8">
         <v>15</v>
       </c>
-      <c r="B16" s="31" t="s">
+      <c r="B16" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="31"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="31"/>
-      <c r="I16" s="31"/>
-      <c r="J16" s="31"/>
-      <c r="K16" s="31"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="27"/>
       <c r="L16" s="1"/>
-      <c r="M16" s="30"/>
+      <c r="M16" s="24"/>
       <c r="N16" s="13" t="s">
-        <v>84</v>
+        <v>107</v>
       </c>
       <c r="O16" s="13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="P16" s="1"/>
     </row>
-    <row r="17" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="8">
         <v>16</v>
       </c>
@@ -1653,47 +1668,45 @@
       <c r="I17" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="K17" s="18"/>
+      <c r="K17" s="17"/>
       <c r="L17" s="1"/>
-      <c r="M17" s="30"/>
-      <c r="N17" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="O17" s="23" t="s">
-        <v>90</v>
+      <c r="M17" s="24"/>
+      <c r="N17" s="41" t="s">
+        <v>84</v>
+      </c>
+      <c r="O17" s="42" t="s">
+        <v>89</v>
       </c>
       <c r="P17" s="1"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="8">
         <v>17</v>
       </c>
       <c r="B18" s="1">
         <v>9</v>
       </c>
-      <c r="C18" s="33" t="s">
+      <c r="C18" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="D18" s="34"/>
+      <c r="D18" s="31"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
-      <c r="J18" s="32" t="s">
+      <c r="J18" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="K18" s="39" t="s">
+      <c r="K18" s="36" t="s">
         <v>8</v>
       </c>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
-      <c r="N18" s="1">
-        <v>15</v>
-      </c>
-      <c r="O18" s="1">
-        <v>10</v>
-      </c>
+      <c r="N18" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="O18" s="43"/>
       <c r="P18" s="1"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.3">
@@ -1703,19 +1716,23 @@
       <c r="B19" s="1">
         <v>10</v>
       </c>
-      <c r="C19" s="35"/>
-      <c r="D19" s="36"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="33"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
-      <c r="J19" s="32"/>
-      <c r="K19" s="39"/>
+      <c r="J19" s="29"/>
+      <c r="K19" s="36"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
-      <c r="N19" s="1"/>
-      <c r="O19" s="1"/>
+      <c r="N19" s="41">
+        <v>17</v>
+      </c>
+      <c r="O19" s="41">
+        <v>10</v>
+      </c>
       <c r="P19" s="1"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.3">
@@ -1725,15 +1742,15 @@
       <c r="B20" s="1">
         <v>11</v>
       </c>
-      <c r="C20" s="35"/>
-      <c r="D20" s="36"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="33"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
-      <c r="J20" s="32"/>
-      <c r="K20" s="39"/>
+      <c r="J20" s="29"/>
+      <c r="K20" s="36"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
@@ -1747,15 +1764,15 @@
       <c r="B21" s="1">
         <v>6</v>
       </c>
-      <c r="C21" s="35"/>
-      <c r="D21" s="36"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="33"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
-      <c r="J21" s="32"/>
-      <c r="K21" s="39"/>
+      <c r="J21" s="29"/>
+      <c r="K21" s="36"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
@@ -1769,15 +1786,15 @@
       <c r="B22" s="1">
         <v>7</v>
       </c>
-      <c r="C22" s="35"/>
-      <c r="D22" s="36"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="33"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
-      <c r="J22" s="32"/>
-      <c r="K22" s="39"/>
+      <c r="J22" s="29"/>
+      <c r="K22" s="36"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
@@ -1791,15 +1808,15 @@
       <c r="B23" s="1">
         <v>8</v>
       </c>
-      <c r="C23" s="37"/>
-      <c r="D23" s="38"/>
+      <c r="C23" s="34"/>
+      <c r="D23" s="35"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
-      <c r="J23" s="32"/>
-      <c r="K23" s="39"/>
+      <c r="J23" s="29"/>
+      <c r="K23" s="36"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
@@ -1813,10 +1830,10 @@
       <c r="B24" s="1">
         <v>15</v>
       </c>
-      <c r="C24" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="D24" s="20" t="s">
+      <c r="C24" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="19" t="s">
         <v>7</v>
       </c>
       <c r="E24" s="1" t="s">
@@ -1832,7 +1849,7 @@
       <c r="I24" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="K24" s="19"/>
+      <c r="K24" s="18"/>
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
@@ -1846,10 +1863,10 @@
       <c r="B25" s="1">
         <v>2</v>
       </c>
-      <c r="C25" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="D25" s="20" t="s">
+      <c r="C25" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="19" t="s">
         <v>7</v>
       </c>
       <c r="E25" s="1" t="s">
@@ -1863,7 +1880,9 @@
         <v>50</v>
       </c>
       <c r="I25" s="1"/>
-      <c r="K25" s="19"/>
+      <c r="K25" s="18" t="s">
+        <v>106</v>
+      </c>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
@@ -1877,10 +1896,10 @@
       <c r="B26" s="10">
         <v>0</v>
       </c>
-      <c r="C26" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="D26" s="21" t="s">
+      <c r="C26" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="20" t="s">
         <v>7</v>
       </c>
       <c r="E26" s="10" t="s">
@@ -1897,7 +1916,7 @@
       <c r="J26" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="K26" s="19"/>
+      <c r="K26" s="18"/>
       <c r="L26" s="10"/>
       <c r="M26" s="10"/>
       <c r="N26" s="10"/>
@@ -1928,8 +1947,8 @@
         <v>55</v>
       </c>
       <c r="I27" s="1"/>
-      <c r="K27" s="19" t="s">
-        <v>101</v>
+      <c r="K27" s="18" t="s">
+        <v>100</v>
       </c>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
@@ -1955,8 +1974,8 @@
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
-      <c r="K28" s="19" t="s">
-        <v>103</v>
+      <c r="K28" s="18" t="s">
+        <v>102</v>
       </c>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
@@ -1982,8 +2001,8 @@
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
-      <c r="K29" s="19" t="s">
-        <v>94</v>
+      <c r="K29" s="18" t="s">
+        <v>93</v>
       </c>
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
@@ -2011,8 +2030,8 @@
       <c r="I30" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="K30" s="19" t="s">
-        <v>96</v>
+      <c r="K30" s="18" t="s">
+        <v>95</v>
       </c>
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
@@ -2040,8 +2059,8 @@
       <c r="I31" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="K31" s="19" t="s">
-        <v>97</v>
+      <c r="K31" s="18" t="s">
+        <v>96</v>
       </c>
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
@@ -2069,8 +2088,8 @@
       <c r="I32" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="K32" s="19" t="s">
-        <v>98</v>
+      <c r="K32" s="18" t="s">
+        <v>97</v>
       </c>
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
@@ -2082,18 +2101,18 @@
       <c r="A33" s="8">
         <v>32</v>
       </c>
-      <c r="B33" s="29" t="s">
+      <c r="B33" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="C33" s="29"/>
-      <c r="D33" s="29"/>
-      <c r="E33" s="29"/>
-      <c r="F33" s="29"/>
-      <c r="G33" s="29"/>
-      <c r="H33" s="29"/>
-      <c r="I33" s="29"/>
-      <c r="J33" s="29"/>
-      <c r="K33" s="29"/>
+      <c r="C33" s="28"/>
+      <c r="D33" s="28"/>
+      <c r="E33" s="28"/>
+      <c r="F33" s="28"/>
+      <c r="G33" s="28"/>
+      <c r="H33" s="28"/>
+      <c r="I33" s="28"/>
+      <c r="J33" s="28"/>
+      <c r="K33" s="28"/>
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
       <c r="N33" s="1"/>
@@ -2120,7 +2139,7 @@
       <c r="I34" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="K34" s="17"/>
+      <c r="K34" s="16"/>
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
       <c r="N34" s="1"/>
@@ -2150,8 +2169,8 @@
       <c r="J35" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="K35" s="40" t="s">
-        <v>95</v>
+      <c r="K35" s="37" t="s">
+        <v>94</v>
       </c>
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
@@ -2182,7 +2201,7 @@
       <c r="J36" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="K36" s="41"/>
+      <c r="K36" s="38"/>
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
       <c r="N36" s="1"/>
@@ -2209,8 +2228,8 @@
       <c r="I37" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="K37" s="17" t="s">
-        <v>99</v>
+      <c r="K37" s="16" t="s">
+        <v>98</v>
       </c>
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
@@ -2238,8 +2257,8 @@
       <c r="I38" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="K38" s="17" t="s">
-        <v>102</v>
+      <c r="K38" s="16" t="s">
+        <v>101</v>
       </c>
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
@@ -2251,18 +2270,18 @@
       <c r="A39" s="8">
         <v>38</v>
       </c>
-      <c r="B39" s="31" t="s">
+      <c r="B39" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="C39" s="31"/>
-      <c r="D39" s="31"/>
-      <c r="E39" s="31"/>
-      <c r="F39" s="31"/>
-      <c r="G39" s="31"/>
-      <c r="H39" s="31"/>
-      <c r="I39" s="31"/>
-      <c r="J39" s="31"/>
-      <c r="K39" s="31"/>
+      <c r="C39" s="27"/>
+      <c r="D39" s="27"/>
+      <c r="E39" s="27"/>
+      <c r="F39" s="27"/>
+      <c r="G39" s="27"/>
+      <c r="H39" s="27"/>
+      <c r="I39" s="27"/>
+      <c r="J39" s="27"/>
+      <c r="K39" s="27"/>
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
       <c r="N39" s="1"/>
@@ -3062,6 +3081,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="B2:K2"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="B4:K4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
     <mergeCell ref="M13:M17"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="B16:K16"/>
@@ -3071,12 +3096,6 @@
     <mergeCell ref="C18:D23"/>
     <mergeCell ref="K18:K23"/>
     <mergeCell ref="K35:K36"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="B2:K2"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="B4:K4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Uso del termometro Tambien he cambiado el nombre de una libreria por errores en el codigo
</commit_message>
<xml_diff>
--- a/Datasheets/ESP CONTROLADOR.xlsx
+++ b/Datasheets/ESP CONTROLADOR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uses0-my.sharepoint.com/personal/serparram_alum_us_es/Documents/Escritorio/Tercero/SegundoCuatri/Proyectos integrados/pi01/Datasheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="78" documentId="8_{D3A0FABF-8483-46B0-83EF-1E4F1725AC99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E8D103F8-0D86-434D-BF50-AC83C5DB5F82}"/>
+  <xr:revisionPtr revIDLastSave="90" documentId="8_{D3A0FABF-8483-46B0-83EF-1E4F1725AC99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F7CF8CEC-5484-40B5-94D1-8FB758D58D37}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{121CA96C-2885-4729-A560-A640673F77D6}"/>
   </bookViews>
@@ -350,9 +350,6 @@
     <t>Boton apagado</t>
   </si>
   <si>
-    <t>2 Input</t>
-  </si>
-  <si>
     <t>Libres</t>
   </si>
   <si>
@@ -368,7 +365,10 @@
     <t>Bomba agua</t>
   </si>
   <si>
-    <t>7 I/O</t>
+    <t>6 I/O</t>
+  </si>
+  <si>
+    <t>3 Input</t>
   </si>
 </sst>
 </file>
@@ -653,7 +653,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -724,21 +724,28 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -769,19 +776,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1123,7 +1118,7 @@
   <dimension ref="A1:P83"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N27" sqref="N27"/>
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1185,18 +1180,18 @@
       <c r="A2" s="8">
         <v>1</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
       <c r="L2" s="1"/>
       <c r="M2" s="2"/>
       <c r="N2" s="1" t="s">
@@ -1209,18 +1204,18 @@
       <c r="A3" s="8">
         <v>2</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="40"/>
-      <c r="J3" s="40"/>
-      <c r="K3" s="40"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
       <c r="L3" s="1"/>
       <c r="M3" s="3"/>
       <c r="N3" s="1" t="s">
@@ -1233,18 +1228,18 @@
       <c r="A4" s="8">
         <v>3</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28"/>
-      <c r="J4" s="28"/>
-      <c r="K4" s="28"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="29"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
@@ -1271,12 +1266,10 @@
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
-      <c r="K5" s="16" t="s">
-        <v>90</v>
-      </c>
+      <c r="K5" s="42"/>
       <c r="L5" s="1"/>
       <c r="M5" s="23" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
@@ -1307,7 +1300,7 @@
       </c>
       <c r="L6" s="1"/>
       <c r="M6" s="13" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
@@ -1336,7 +1329,7 @@
       <c r="K7" s="16"/>
       <c r="L7" s="1"/>
       <c r="M7" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
@@ -1459,7 +1452,9 @@
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
-      <c r="K11" s="18"/>
+      <c r="K11" s="16" t="s">
+        <v>90</v>
+      </c>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
       <c r="O11" s="1"/>
@@ -1526,7 +1521,7 @@
         <v>99</v>
       </c>
       <c r="L13" s="1"/>
-      <c r="M13" s="24" t="s">
+      <c r="M13" s="30" t="s">
         <v>87</v>
       </c>
       <c r="N13" s="13" t="s">
@@ -1564,10 +1559,10 @@
         <v>67</v>
       </c>
       <c r="K14" s="18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L14" s="1"/>
-      <c r="M14" s="24"/>
+      <c r="M14" s="30"/>
       <c r="N14" s="13" t="s">
         <v>82</v>
       </c>
@@ -1607,7 +1602,7 @@
       </c>
       <c r="K15" s="18"/>
       <c r="L15" s="1"/>
-      <c r="M15" s="24"/>
+      <c r="M15" s="30"/>
       <c r="N15" s="13" t="s">
         <v>83</v>
       </c>
@@ -1620,22 +1615,22 @@
       <c r="A16" s="8">
         <v>15</v>
       </c>
-      <c r="B16" s="27" t="s">
+      <c r="B16" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="27"/>
-      <c r="I16" s="27"/>
-      <c r="J16" s="27"/>
-      <c r="K16" s="27"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="31"/>
+      <c r="G16" s="31"/>
+      <c r="H16" s="31"/>
+      <c r="I16" s="31"/>
+      <c r="J16" s="31"/>
+      <c r="K16" s="31"/>
       <c r="L16" s="1"/>
-      <c r="M16" s="24"/>
+      <c r="M16" s="30"/>
       <c r="N16" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="O16" s="13" t="s">
         <v>88</v>
@@ -1670,11 +1665,11 @@
       </c>
       <c r="K17" s="17"/>
       <c r="L17" s="1"/>
-      <c r="M17" s="24"/>
-      <c r="N17" s="41" t="s">
+      <c r="M17" s="30"/>
+      <c r="N17" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="O17" s="42" t="s">
+      <c r="O17" s="13" t="s">
         <v>89</v>
       </c>
       <c r="P17" s="1"/>
@@ -1686,27 +1681,27 @@
       <c r="B18" s="1">
         <v>9</v>
       </c>
-      <c r="C18" s="30" t="s">
+      <c r="C18" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="D18" s="31"/>
+      <c r="D18" s="34"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
-      <c r="J18" s="29" t="s">
+      <c r="J18" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="K18" s="36" t="s">
+      <c r="K18" s="39" t="s">
         <v>8</v>
       </c>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
       <c r="N18" s="22" t="s">
-        <v>108</v>
-      </c>
-      <c r="O18" s="43"/>
+        <v>107</v>
+      </c>
+      <c r="O18" s="24"/>
       <c r="P18" s="1"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.3">
@@ -1716,21 +1711,21 @@
       <c r="B19" s="1">
         <v>10</v>
       </c>
-      <c r="C19" s="32"/>
-      <c r="D19" s="33"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="36"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
-      <c r="J19" s="29"/>
-      <c r="K19" s="36"/>
+      <c r="J19" s="32"/>
+      <c r="K19" s="39"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
-      <c r="N19" s="41">
+      <c r="N19" s="1">
         <v>17</v>
       </c>
-      <c r="O19" s="41">
+      <c r="O19" s="1">
         <v>10</v>
       </c>
       <c r="P19" s="1"/>
@@ -1742,15 +1737,15 @@
       <c r="B20" s="1">
         <v>11</v>
       </c>
-      <c r="C20" s="32"/>
-      <c r="D20" s="33"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="36"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
-      <c r="J20" s="29"/>
-      <c r="K20" s="36"/>
+      <c r="J20" s="32"/>
+      <c r="K20" s="39"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
@@ -1764,15 +1759,15 @@
       <c r="B21" s="1">
         <v>6</v>
       </c>
-      <c r="C21" s="32"/>
-      <c r="D21" s="33"/>
+      <c r="C21" s="35"/>
+      <c r="D21" s="36"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
-      <c r="J21" s="29"/>
-      <c r="K21" s="36"/>
+      <c r="J21" s="32"/>
+      <c r="K21" s="39"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
@@ -1786,15 +1781,15 @@
       <c r="B22" s="1">
         <v>7</v>
       </c>
-      <c r="C22" s="32"/>
-      <c r="D22" s="33"/>
+      <c r="C22" s="35"/>
+      <c r="D22" s="36"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
-      <c r="J22" s="29"/>
-      <c r="K22" s="36"/>
+      <c r="J22" s="32"/>
+      <c r="K22" s="39"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
@@ -1808,15 +1803,15 @@
       <c r="B23" s="1">
         <v>8</v>
       </c>
-      <c r="C23" s="34"/>
-      <c r="D23" s="35"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="38"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
-      <c r="J23" s="29"/>
-      <c r="K23" s="36"/>
+      <c r="J23" s="32"/>
+      <c r="K23" s="39"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
@@ -1881,7 +1876,7 @@
       </c>
       <c r="I25" s="1"/>
       <c r="K25" s="18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
@@ -2101,18 +2096,18 @@
       <c r="A33" s="8">
         <v>32</v>
       </c>
-      <c r="B33" s="28" t="s">
+      <c r="B33" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="C33" s="28"/>
-      <c r="D33" s="28"/>
-      <c r="E33" s="28"/>
-      <c r="F33" s="28"/>
-      <c r="G33" s="28"/>
-      <c r="H33" s="28"/>
-      <c r="I33" s="28"/>
-      <c r="J33" s="28"/>
-      <c r="K33" s="28"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="29"/>
+      <c r="E33" s="29"/>
+      <c r="F33" s="29"/>
+      <c r="G33" s="29"/>
+      <c r="H33" s="29"/>
+      <c r="I33" s="29"/>
+      <c r="J33" s="29"/>
+      <c r="K33" s="29"/>
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
       <c r="N33" s="1"/>
@@ -2169,7 +2164,7 @@
       <c r="J35" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="K35" s="37" t="s">
+      <c r="K35" s="40" t="s">
         <v>94</v>
       </c>
       <c r="L35" s="1"/>
@@ -2201,7 +2196,7 @@
       <c r="J36" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="K36" s="38"/>
+      <c r="K36" s="41"/>
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
       <c r="N36" s="1"/>
@@ -2270,18 +2265,18 @@
       <c r="A39" s="8">
         <v>38</v>
       </c>
-      <c r="B39" s="27" t="s">
+      <c r="B39" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="C39" s="27"/>
-      <c r="D39" s="27"/>
-      <c r="E39" s="27"/>
-      <c r="F39" s="27"/>
-      <c r="G39" s="27"/>
-      <c r="H39" s="27"/>
-      <c r="I39" s="27"/>
-      <c r="J39" s="27"/>
-      <c r="K39" s="27"/>
+      <c r="C39" s="31"/>
+      <c r="D39" s="31"/>
+      <c r="E39" s="31"/>
+      <c r="F39" s="31"/>
+      <c r="G39" s="31"/>
+      <c r="H39" s="31"/>
+      <c r="I39" s="31"/>
+      <c r="J39" s="31"/>
+      <c r="K39" s="31"/>
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
       <c r="N39" s="1"/>
@@ -3081,12 +3076,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="B2:K2"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="B4:K4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
     <mergeCell ref="M13:M17"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="B16:K16"/>
@@ -3096,6 +3085,12 @@
     <mergeCell ref="C18:D23"/>
     <mergeCell ref="K18:K23"/>
     <mergeCell ref="K35:K36"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="B2:K2"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="B4:K4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Creacion de carpetas para ambos esp32
</commit_message>
<xml_diff>
--- a/Datasheets/ESP CONTROLADOR.xlsx
+++ b/Datasheets/ESP CONTROLADOR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uses0-my.sharepoint.com/personal/serparram_alum_us_es/Documents/Escritorio/Tercero/SegundoCuatri/Proyectos integrados/pi01/Datasheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="90" documentId="8_{D3A0FABF-8483-46B0-83EF-1E4F1725AC99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F7CF8CEC-5484-40B5-94D1-8FB758D58D37}"/>
+  <xr:revisionPtr revIDLastSave="110" documentId="8_{D3A0FABF-8483-46B0-83EF-1E4F1725AC99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4DBF68B5-F821-4C30-9D1C-CC330A9F1348}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{121CA96C-2885-4729-A560-A640673F77D6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="114">
   <si>
     <t>INPUT</t>
   </si>
@@ -212,9 +212,6 @@
     <t>ADC2_CH0</t>
   </si>
   <si>
-    <t>Transmisión serie</t>
-  </si>
-  <si>
     <t>fino</t>
   </si>
   <si>
@@ -369,6 +366,18 @@
   </si>
   <si>
     <t>3 Input</t>
+  </si>
+  <si>
+    <t>Comunicación ordenador</t>
+  </si>
+  <si>
+    <t>Monitor serie</t>
+  </si>
+  <si>
+    <t>UART (RX)</t>
+  </si>
+  <si>
+    <t>UART (TX)</t>
   </si>
 </sst>
 </file>
@@ -653,7 +662,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -725,58 +734,61 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1118,7 +1130,7 @@
   <dimension ref="A1:P83"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1129,14 +1141,14 @@
     <col min="8" max="8" width="10.6640625" customWidth="1"/>
     <col min="9" max="9" width="15.109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="62.77734375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.44140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="24.5546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="20.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>2</v>
@@ -1160,18 +1172,18 @@
         <v>17</v>
       </c>
       <c r="I1" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="J1" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="K1" s="7" t="s">
         <v>71</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>72</v>
       </c>
       <c r="L1" s="1"/>
       <c r="M1" s="9"/>
       <c r="N1" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
@@ -1180,22 +1192,22 @@
       <c r="A2" s="8">
         <v>1</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="41"/>
       <c r="L2" s="1"/>
       <c r="M2" s="2"/>
       <c r="N2" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
@@ -1204,22 +1216,22 @@
       <c r="A3" s="8">
         <v>2</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="42"/>
+      <c r="K3" s="42"/>
       <c r="L3" s="1"/>
       <c r="M3" s="3"/>
       <c r="N3" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
@@ -1228,18 +1240,18 @@
       <c r="A4" s="8">
         <v>3</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="29"/>
-      <c r="K4" s="29"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="30"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
@@ -1253,10 +1265,10 @@
       <c r="B5" s="1">
         <v>36</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="26"/>
+      <c r="D5" s="28"/>
       <c r="E5" s="1" t="s">
         <v>12</v>
       </c>
@@ -1266,10 +1278,10 @@
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
-      <c r="K5" s="42"/>
+      <c r="K5" s="25"/>
       <c r="L5" s="1"/>
       <c r="M5" s="23" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
@@ -1282,10 +1294,10 @@
       <c r="B6" s="1">
         <v>39</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="26"/>
+      <c r="D6" s="28"/>
       <c r="E6" s="1" t="s">
         <v>13</v>
       </c>
@@ -1296,11 +1308,11 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="K6" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L6" s="1"/>
       <c r="M6" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
@@ -1313,10 +1325,10 @@
       <c r="B7" s="1">
         <v>34</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="26"/>
+      <c r="D7" s="28"/>
       <c r="E7" s="1" t="s">
         <v>14</v>
       </c>
@@ -1329,7 +1341,7 @@
       <c r="K7" s="16"/>
       <c r="L7" s="1"/>
       <c r="M7" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
@@ -1342,10 +1354,10 @@
       <c r="B8" s="1">
         <v>35</v>
       </c>
-      <c r="C8" s="25" t="s">
+      <c r="C8" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="26"/>
+      <c r="D8" s="28"/>
       <c r="E8" s="1" t="s">
         <v>15</v>
       </c>
@@ -1387,7 +1399,7 @@
       </c>
       <c r="I9" s="1"/>
       <c r="K9" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
@@ -1420,7 +1432,7 @@
       </c>
       <c r="I10" s="1"/>
       <c r="K10" s="21" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
@@ -1453,7 +1465,7 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="K11" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
@@ -1488,7 +1500,7 @@
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
       <c r="N12" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="O12" s="14" t="s">
         <v>0</v>
@@ -1518,17 +1530,17 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="K13" s="18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L13" s="1"/>
-      <c r="M13" s="30" t="s">
-        <v>87</v>
+      <c r="M13" s="26" t="s">
+        <v>86</v>
       </c>
       <c r="N13" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="O13" s="13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="P13" s="1"/>
     </row>
@@ -1556,18 +1568,18 @@
         <v>44</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K14" s="18" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="L14" s="1"/>
-      <c r="M14" s="30"/>
+      <c r="M14" s="26"/>
       <c r="N14" s="13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="P14" s="1"/>
     </row>
@@ -1595,19 +1607,19 @@
         <v>43</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K15" s="18"/>
       <c r="L15" s="1"/>
-      <c r="M15" s="30"/>
+      <c r="M15" s="26"/>
       <c r="N15" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O15" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="P15" s="1"/>
     </row>
@@ -1615,25 +1627,25 @@
       <c r="A16" s="8">
         <v>15</v>
       </c>
-      <c r="B16" s="31" t="s">
+      <c r="B16" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="31"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="31"/>
-      <c r="I16" s="31"/>
-      <c r="J16" s="31"/>
-      <c r="K16" s="31"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
+      <c r="K16" s="29"/>
       <c r="L16" s="1"/>
-      <c r="M16" s="30"/>
+      <c r="M16" s="26"/>
       <c r="N16" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="O16" s="13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="P16" s="1"/>
     </row>
@@ -1661,16 +1673,16 @@
         <v>42</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K17" s="17"/>
       <c r="L17" s="1"/>
-      <c r="M17" s="30"/>
+      <c r="M17" s="26"/>
       <c r="N17" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O17" s="13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="P17" s="1"/>
     </row>
@@ -1681,25 +1693,25 @@
       <c r="B18" s="1">
         <v>9</v>
       </c>
-      <c r="C18" s="33" t="s">
+      <c r="C18" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="D18" s="34"/>
+      <c r="D18" s="33"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
-      <c r="J18" s="32" t="s">
-        <v>76</v>
-      </c>
-      <c r="K18" s="39" t="s">
+      <c r="J18" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="K18" s="38" t="s">
         <v>8</v>
       </c>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
       <c r="N18" s="22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="O18" s="24"/>
       <c r="P18" s="1"/>
@@ -1711,15 +1723,15 @@
       <c r="B19" s="1">
         <v>10</v>
       </c>
-      <c r="C19" s="35"/>
-      <c r="D19" s="36"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="35"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
-      <c r="J19" s="32"/>
-      <c r="K19" s="39"/>
+      <c r="J19" s="31"/>
+      <c r="K19" s="38"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
       <c r="N19" s="1">
@@ -1737,15 +1749,15 @@
       <c r="B20" s="1">
         <v>11</v>
       </c>
-      <c r="C20" s="35"/>
-      <c r="D20" s="36"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="35"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
-      <c r="J20" s="32"/>
-      <c r="K20" s="39"/>
+      <c r="J20" s="31"/>
+      <c r="K20" s="38"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
@@ -1759,15 +1771,15 @@
       <c r="B21" s="1">
         <v>6</v>
       </c>
-      <c r="C21" s="35"/>
-      <c r="D21" s="36"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="35"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
-      <c r="J21" s="32"/>
-      <c r="K21" s="39"/>
+      <c r="J21" s="31"/>
+      <c r="K21" s="38"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
@@ -1781,15 +1793,15 @@
       <c r="B22" s="1">
         <v>7</v>
       </c>
-      <c r="C22" s="35"/>
-      <c r="D22" s="36"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="35"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
-      <c r="J22" s="32"/>
-      <c r="K22" s="39"/>
+      <c r="J22" s="31"/>
+      <c r="K22" s="38"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
@@ -1803,15 +1815,15 @@
       <c r="B23" s="1">
         <v>8</v>
       </c>
-      <c r="C23" s="37"/>
-      <c r="D23" s="38"/>
+      <c r="C23" s="36"/>
+      <c r="D23" s="37"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
-      <c r="J23" s="32"/>
-      <c r="K23" s="39"/>
+      <c r="J23" s="31"/>
+      <c r="K23" s="38"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
@@ -1842,9 +1854,11 @@
         <v>48</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="K24" s="18"/>
+        <v>65</v>
+      </c>
+      <c r="K24" s="18" t="s">
+        <v>101</v>
+      </c>
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
@@ -1876,7 +1890,7 @@
       </c>
       <c r="I25" s="1"/>
       <c r="K25" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
@@ -1909,7 +1923,7 @@
       </c>
       <c r="I26" s="10"/>
       <c r="J26" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K26" s="18"/>
       <c r="L26" s="10"/>
@@ -1943,7 +1957,7 @@
       </c>
       <c r="I27" s="1"/>
       <c r="K27" s="18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
@@ -1968,9 +1982,11 @@
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-      <c r="K28" s="18" t="s">
-        <v>102</v>
+      <c r="I28" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="K28" s="43" t="s">
+        <v>93</v>
       </c>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
@@ -1995,10 +2011,10 @@
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-      <c r="K29" s="18" t="s">
-        <v>93</v>
-      </c>
+      <c r="I29" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="K29" s="43"/>
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
       <c r="N29" s="1"/>
@@ -2023,10 +2039,10 @@
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K30" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
@@ -2052,10 +2068,10 @@
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K31" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
@@ -2081,10 +2097,10 @@
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K32" s="18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
@@ -2096,18 +2112,18 @@
       <c r="A33" s="8">
         <v>32</v>
       </c>
-      <c r="B33" s="29" t="s">
+      <c r="B33" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="C33" s="29"/>
-      <c r="D33" s="29"/>
-      <c r="E33" s="29"/>
-      <c r="F33" s="29"/>
-      <c r="G33" s="29"/>
-      <c r="H33" s="29"/>
-      <c r="I33" s="29"/>
-      <c r="J33" s="29"/>
-      <c r="K33" s="29"/>
+      <c r="C33" s="30"/>
+      <c r="D33" s="30"/>
+      <c r="E33" s="30"/>
+      <c r="F33" s="30"/>
+      <c r="G33" s="30"/>
+      <c r="H33" s="30"/>
+      <c r="I33" s="30"/>
+      <c r="J33" s="30"/>
+      <c r="K33" s="30"/>
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
       <c r="N33" s="1"/>
@@ -2132,9 +2148,11 @@
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="K34" s="16"/>
+        <v>60</v>
+      </c>
+      <c r="K34" s="18" t="s">
+        <v>92</v>
+      </c>
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
       <c r="N34" s="1"/>
@@ -2159,13 +2177,13 @@
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1" t="s">
-        <v>58</v>
+        <v>111</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="K35" s="40" t="s">
-        <v>94</v>
+        <v>76</v>
+      </c>
+      <c r="K35" s="39" t="s">
+        <v>110</v>
       </c>
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
@@ -2191,12 +2209,12 @@
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
       <c r="I36" s="1" t="s">
-        <v>58</v>
+        <v>111</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K36" s="41"/>
+        <v>77</v>
+      </c>
+      <c r="K36" s="40"/>
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
       <c r="N36" s="1"/>
@@ -2221,10 +2239,10 @@
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
       <c r="I37" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K37" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
@@ -2250,10 +2268,10 @@
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
       <c r="I38" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K38" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
@@ -2265,18 +2283,18 @@
       <c r="A39" s="8">
         <v>38</v>
       </c>
-      <c r="B39" s="31" t="s">
+      <c r="B39" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="C39" s="31"/>
-      <c r="D39" s="31"/>
-      <c r="E39" s="31"/>
-      <c r="F39" s="31"/>
-      <c r="G39" s="31"/>
-      <c r="H39" s="31"/>
-      <c r="I39" s="31"/>
-      <c r="J39" s="31"/>
-      <c r="K39" s="31"/>
+      <c r="C39" s="29"/>
+      <c r="D39" s="29"/>
+      <c r="E39" s="29"/>
+      <c r="F39" s="29"/>
+      <c r="G39" s="29"/>
+      <c r="H39" s="29"/>
+      <c r="I39" s="29"/>
+      <c r="J39" s="29"/>
+      <c r="K39" s="29"/>
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
       <c r="N39" s="1"/>
@@ -3075,7 +3093,13 @@
       <c r="P83" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="16">
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="B2:K2"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="B4:K4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
     <mergeCell ref="M13:M17"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="B16:K16"/>
@@ -3085,12 +3109,7 @@
     <mergeCell ref="C18:D23"/>
     <mergeCell ref="K18:K23"/>
     <mergeCell ref="K35:K36"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="B2:K2"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="B4:K4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="K28:K29"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Usos de la UART y maquina de estados
</commit_message>
<xml_diff>
--- a/Datasheets/ESP CONTROLADOR.xlsx
+++ b/Datasheets/ESP CONTROLADOR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uses0-my.sharepoint.com/personal/serparram_alum_us_es/Documents/Escritorio/Tercero/SegundoCuatri/Proyectos integrados/pi01/Datasheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="110" documentId="8_{D3A0FABF-8483-46B0-83EF-1E4F1725AC99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4DBF68B5-F821-4C30-9D1C-CC330A9F1348}"/>
+  <xr:revisionPtr revIDLastSave="111" documentId="8_{D3A0FABF-8483-46B0-83EF-1E4F1725AC99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6BD7AD96-8C7F-4953-8AA9-3903F59F1AF9}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{121CA96C-2885-4729-A560-A640673F77D6}"/>
   </bookViews>
@@ -362,9 +362,6 @@
     <t>Bomba agua</t>
   </si>
   <si>
-    <t>6 I/O</t>
-  </si>
-  <si>
     <t>3 Input</t>
   </si>
   <si>
@@ -378,6 +375,9 @@
   </si>
   <si>
     <t>UART (TX)</t>
+  </si>
+  <si>
+    <t>4 I/O</t>
   </si>
 </sst>
 </file>
@@ -735,21 +735,27 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -779,12 +785,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1130,7 +1130,7 @@
   <dimension ref="A1:P83"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1192,18 +1192,18 @@
       <c r="A2" s="8">
         <v>1</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41"/>
-      <c r="K2" s="41"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
       <c r="L2" s="1"/>
       <c r="M2" s="2"/>
       <c r="N2" s="1" t="s">
@@ -1216,18 +1216,18 @@
       <c r="A3" s="8">
         <v>2</v>
       </c>
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="42"/>
-      <c r="K3" s="42"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
       <c r="L3" s="1"/>
       <c r="M3" s="3"/>
       <c r="N3" s="1" t="s">
@@ -1265,10 +1265,10 @@
       <c r="B5" s="1">
         <v>36</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="28"/>
+      <c r="D5" s="27"/>
       <c r="E5" s="1" t="s">
         <v>12</v>
       </c>
@@ -1294,10 +1294,10 @@
       <c r="B6" s="1">
         <v>39</v>
       </c>
-      <c r="C6" s="27" t="s">
+      <c r="C6" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="28"/>
+      <c r="D6" s="27"/>
       <c r="E6" s="1" t="s">
         <v>13</v>
       </c>
@@ -1312,7 +1312,7 @@
       </c>
       <c r="L6" s="1"/>
       <c r="M6" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
@@ -1325,10 +1325,10 @@
       <c r="B7" s="1">
         <v>34</v>
       </c>
-      <c r="C7" s="27" t="s">
+      <c r="C7" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="28"/>
+      <c r="D7" s="27"/>
       <c r="E7" s="1" t="s">
         <v>14</v>
       </c>
@@ -1341,7 +1341,7 @@
       <c r="K7" s="16"/>
       <c r="L7" s="1"/>
       <c r="M7" s="13" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
@@ -1354,10 +1354,10 @@
       <c r="B8" s="1">
         <v>35</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="28"/>
+      <c r="D8" s="27"/>
       <c r="E8" s="1" t="s">
         <v>15</v>
       </c>
@@ -1533,7 +1533,7 @@
         <v>98</v>
       </c>
       <c r="L13" s="1"/>
-      <c r="M13" s="26" t="s">
+      <c r="M13" s="31" t="s">
         <v>86</v>
       </c>
       <c r="N13" s="13" t="s">
@@ -1574,7 +1574,7 @@
         <v>107</v>
       </c>
       <c r="L14" s="1"/>
-      <c r="M14" s="26"/>
+      <c r="M14" s="31"/>
       <c r="N14" s="13" t="s">
         <v>81</v>
       </c>
@@ -1614,7 +1614,7 @@
       </c>
       <c r="K15" s="18"/>
       <c r="L15" s="1"/>
-      <c r="M15" s="26"/>
+      <c r="M15" s="31"/>
       <c r="N15" s="13" t="s">
         <v>82</v>
       </c>
@@ -1627,20 +1627,20 @@
       <c r="A16" s="8">
         <v>15</v>
       </c>
-      <c r="B16" s="29" t="s">
+      <c r="B16" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="29"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="29"/>
-      <c r="G16" s="29"/>
-      <c r="H16" s="29"/>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
-      <c r="K16" s="29"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="32"/>
+      <c r="J16" s="32"/>
+      <c r="K16" s="32"/>
       <c r="L16" s="1"/>
-      <c r="M16" s="26"/>
+      <c r="M16" s="31"/>
       <c r="N16" s="13" t="s">
         <v>105</v>
       </c>
@@ -1677,7 +1677,7 @@
       </c>
       <c r="K17" s="17"/>
       <c r="L17" s="1"/>
-      <c r="M17" s="26"/>
+      <c r="M17" s="31"/>
       <c r="N17" s="1" t="s">
         <v>83</v>
       </c>
@@ -1693,19 +1693,19 @@
       <c r="B18" s="1">
         <v>9</v>
       </c>
-      <c r="C18" s="32" t="s">
+      <c r="C18" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="D18" s="33"/>
+      <c r="D18" s="35"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
-      <c r="J18" s="31" t="s">
+      <c r="J18" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="K18" s="38" t="s">
+      <c r="K18" s="40" t="s">
         <v>8</v>
       </c>
       <c r="L18" s="1"/>
@@ -1723,15 +1723,15 @@
       <c r="B19" s="1">
         <v>10</v>
       </c>
-      <c r="C19" s="34"/>
-      <c r="D19" s="35"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="37"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
-      <c r="J19" s="31"/>
-      <c r="K19" s="38"/>
+      <c r="J19" s="33"/>
+      <c r="K19" s="40"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
       <c r="N19" s="1">
@@ -1749,15 +1749,15 @@
       <c r="B20" s="1">
         <v>11</v>
       </c>
-      <c r="C20" s="34"/>
-      <c r="D20" s="35"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="37"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
-      <c r="J20" s="31"/>
-      <c r="K20" s="38"/>
+      <c r="J20" s="33"/>
+      <c r="K20" s="40"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
@@ -1771,15 +1771,15 @@
       <c r="B21" s="1">
         <v>6</v>
       </c>
-      <c r="C21" s="34"/>
-      <c r="D21" s="35"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="37"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
-      <c r="J21" s="31"/>
-      <c r="K21" s="38"/>
+      <c r="J21" s="33"/>
+      <c r="K21" s="40"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
@@ -1793,15 +1793,15 @@
       <c r="B22" s="1">
         <v>7</v>
       </c>
-      <c r="C22" s="34"/>
-      <c r="D22" s="35"/>
+      <c r="C22" s="36"/>
+      <c r="D22" s="37"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
-      <c r="J22" s="31"/>
-      <c r="K22" s="38"/>
+      <c r="J22" s="33"/>
+      <c r="K22" s="40"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
@@ -1815,15 +1815,15 @@
       <c r="B23" s="1">
         <v>8</v>
       </c>
-      <c r="C23" s="36"/>
-      <c r="D23" s="37"/>
+      <c r="C23" s="38"/>
+      <c r="D23" s="39"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
-      <c r="J23" s="31"/>
-      <c r="K23" s="38"/>
+      <c r="J23" s="33"/>
+      <c r="K23" s="40"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
@@ -1983,7 +1983,7 @@
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K28" s="43" t="s">
         <v>93</v>
@@ -2012,7 +2012,7 @@
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K29" s="43"/>
       <c r="L29" s="1"/>
@@ -2177,13 +2177,13 @@
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J35" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="K35" s="39" t="s">
-        <v>110</v>
+      <c r="K35" s="41" t="s">
+        <v>109</v>
       </c>
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
@@ -2209,12 +2209,12 @@
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
       <c r="I36" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J36" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="K36" s="40"/>
+      <c r="K36" s="42"/>
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
       <c r="N36" s="1"/>
@@ -2283,18 +2283,18 @@
       <c r="A39" s="8">
         <v>38</v>
       </c>
-      <c r="B39" s="29" t="s">
+      <c r="B39" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="C39" s="29"/>
-      <c r="D39" s="29"/>
-      <c r="E39" s="29"/>
-      <c r="F39" s="29"/>
-      <c r="G39" s="29"/>
-      <c r="H39" s="29"/>
-      <c r="I39" s="29"/>
-      <c r="J39" s="29"/>
-      <c r="K39" s="29"/>
+      <c r="C39" s="32"/>
+      <c r="D39" s="32"/>
+      <c r="E39" s="32"/>
+      <c r="F39" s="32"/>
+      <c r="G39" s="32"/>
+      <c r="H39" s="32"/>
+      <c r="I39" s="32"/>
+      <c r="J39" s="32"/>
+      <c r="K39" s="32"/>
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
       <c r="N39" s="1"/>
@@ -3094,12 +3094,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="B2:K2"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="B4:K4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
     <mergeCell ref="M13:M17"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="B16:K16"/>
@@ -3110,6 +3104,12 @@
     <mergeCell ref="K18:K23"/>
     <mergeCell ref="K35:K36"/>
     <mergeCell ref="K28:K29"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="B2:K2"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="B4:K4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>